<commit_message>
Updated Car Inventory Project.
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\.NET Development II\Final Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A504ABF1-89B8-418B-A678-E29E57000248}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0E5D254-4146-4344-80F6-AB4769E70607}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2370" yWindow="2010" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -57,9 +57,6 @@
     <t>I can save my preferences and track my interactions with the dealership.</t>
   </si>
   <si>
-    <t>Sales Representative</t>
-  </si>
-  <si>
     <t>Manager</t>
   </si>
   <si>
@@ -142,6 +139,9 @@
   </si>
   <si>
     <t xml:space="preserve">I can change my password </t>
+  </si>
+  <si>
+    <t>Sales Representative, Manager</t>
   </si>
 </sst>
 </file>
@@ -472,8 +472,8 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -510,7 +510,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>6</v>
@@ -524,7 +524,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -532,21 +532,21 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -554,37 +554,37 @@
         <v>3</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>8</v>
@@ -595,68 +595,68 @@
     </row>
     <row r="11" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:3" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:3" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:3" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="C14" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="C15" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>